<commit_message>
rigid body bug fixes
</commit_message>
<xml_diff>
--- a/ffxiv_mmd_tools_helper_beta/data/rigid_body.xlsx
+++ b/ffxiv_mmd_tools_helper_beta/data/rigid_body.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMD\ffxiv_mmd_tools_helper\ffxiv_mmd_tools_helper_beta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1E9659-65ED-49D1-8425-69B97804004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873343ED-FB46-4244-95C0-9482DE8A2023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44295" yWindow="4650" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39885" yWindow="4200" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="83">
   <si>
     <t>bone_name</t>
   </si>
@@ -260,6 +260,21 @@
   </si>
   <si>
     <t>j_asi_c_r</t>
+  </si>
+  <si>
+    <t>rigid_body_name</t>
+  </si>
+  <si>
+    <t>upper_body b</t>
+  </si>
+  <si>
+    <t>j_mune_l</t>
+  </si>
+  <si>
+    <t>j_mune_r</t>
+  </si>
+  <si>
+    <t>upper body 2b</t>
   </si>
 </sst>
 </file>
@@ -533,9 +548,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}" name="Table22" displayName="Table22" ref="A1:AH32" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:AH32" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}"/>
-  <tableColumns count="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}" name="Table22" displayName="Table22" ref="A1:AI32" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:AI32" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}"/>
+  <tableColumns count="35">
+    <tableColumn id="6" xr3:uid="{46085F6A-14DA-41C2-880B-EA29369D9E3D}" name="rigid_body_name"/>
     <tableColumn id="3" xr3:uid="{E619AE08-CCC5-4E49-92F3-B342CA7A97F8}" name="bone_name"/>
     <tableColumn id="37" xr3:uid="{C9198B0D-8302-498D-9D2E-2D9754DE85EA}" name="offset_x"/>
     <tableColumn id="38" xr3:uid="{EC4189AE-8CF9-413F-BBCC-922A256DEC18}" name="offset_y"/>
@@ -2253,167 +2269,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D213BE9-EC88-43A5-B10E-7AC8A26A2FF6}">
-  <dimension ref="A1:AH32"/>
+  <dimension ref="A1:AI32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:J18"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" customWidth="1"/>
-    <col min="22" max="22" width="9.28515625" customWidth="1"/>
-    <col min="26" max="27" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" customWidth="1"/>
-    <col min="30" max="30" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" customWidth="1"/>
+    <col min="28" max="29" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AD1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AE1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AF1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AI1" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6"/>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="12">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="D2" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="6">
-        <v>0.06</v>
-      </c>
-      <c r="J2" s="6"/>
+      <c r="J2" s="6">
+        <v>0.08</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -2421,61 +2446,64 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="6">
-        <v>1</v>
-      </c>
-      <c r="S2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6">
+        <v>1</v>
+      </c>
       <c r="T2" s="6"/>
-      <c r="U2" s="6">
-        <v>0</v>
-      </c>
+      <c r="U2" s="6"/>
       <c r="V2" s="6">
         <v>0</v>
       </c>
       <c r="W2" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="X2" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="X2" s="6">
+        <v>0.5</v>
+      </c>
       <c r="Y2" s="6"/>
-      <c r="Z2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6">
+        <v>0</v>
+      </c>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="AD2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6">
+        <v>0.5</v>
+      </c>
       <c r="AE2" s="6"/>
-      <c r="AF2" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="7"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="7"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0.05</v>
       </c>
-      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -2483,1306 +2511,1483 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2">
-        <v>1</v>
-      </c>
-      <c r="S3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
       <c r="T3" s="2"/>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
+      <c r="U3" s="2"/>
       <c r="V3" s="2">
         <v>0</v>
       </c>
       <c r="W3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="X3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0.5</v>
+      </c>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2">
+        <v>0</v>
+      </c>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AD3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2">
+        <v>0.5</v>
+      </c>
       <c r="AE3" s="2"/>
-      <c r="AF3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="3"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="3"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I4">
+      <c r="J4" s="6">
         <v>0.06</v>
       </c>
-      <c r="J4">
+      <c r="K4" s="6">
         <v>0.12</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
+      <c r="S4">
+        <v>1</v>
       </c>
       <c r="V4">
         <v>0</v>
       </c>
       <c r="W4">
-        <v>0.5</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0.5</v>
-      </c>
-      <c r="AF4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0.5</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0.5</v>
+      </c>
+      <c r="AG4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I5">
+      <c r="J5" s="6">
         <v>0.1</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
+      <c r="K5" s="6"/>
+      <c r="S5">
+        <v>1</v>
       </c>
       <c r="V5">
         <v>0</v>
       </c>
       <c r="W5">
-        <v>0.5</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0.5</v>
-      </c>
-      <c r="AF5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0.5</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0.5</v>
+      </c>
+      <c r="AG5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I6">
+      <c r="J6" s="6">
         <v>0.06</v>
       </c>
-      <c r="J6">
+      <c r="K6" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
+      <c r="S6">
+        <v>1</v>
       </c>
       <c r="V6">
         <v>0</v>
       </c>
       <c r="W6">
-        <v>0.5</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0.5</v>
-      </c>
-      <c r="AF6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0.5</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0.5</v>
+      </c>
+      <c r="AG6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I7">
+      <c r="J7" s="6">
         <v>0.08</v>
       </c>
-      <c r="J7">
+      <c r="K7" s="6">
         <v>0.15</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
+      <c r="S7">
+        <v>1</v>
       </c>
       <c r="V7">
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0.5</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>0.5</v>
-      </c>
-      <c r="AF7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0.5</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0.5</v>
+      </c>
+      <c r="AG7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="B8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I8">
+      <c r="J8" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J8">
+      <c r="K8" s="6">
         <v>0.03</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
+      <c r="S8">
+        <v>1</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0.5</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0.5</v>
-      </c>
-      <c r="AF8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0.5</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0.5</v>
+      </c>
+      <c r="AG8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
+        <v>-0.05</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J9">
+      <c r="J9" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="K9" s="6">
         <v>0.03</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
+      <c r="S9">
+        <v>1</v>
       </c>
       <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0.5</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>0.5</v>
-      </c>
-      <c r="AF9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="12">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0.5</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0.5</v>
+      </c>
+      <c r="AG9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-0.05</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I10">
+      <c r="J10" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="R10">
+      <c r="K10" s="6"/>
+      <c r="S10">
         <v>0.1</v>
       </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
       <c r="V10">
         <v>0</v>
       </c>
       <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
         <v>0.45</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>17</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>0.999</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <v>0.999</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="12">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-0.01</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-0.05</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I11">
+      <c r="J11" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="R11">
+      <c r="K11" s="6"/>
+      <c r="S11">
         <v>0.1</v>
       </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
       <c r="V11">
         <v>0</v>
       </c>
       <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
         <v>0.45</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>17</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>0.999</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>0.999</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="B12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I12">
+      <c r="J12" s="6">
         <v>0.1</v>
       </c>
-      <c r="J12">
+      <c r="K12" s="6">
         <v>0.08</v>
       </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
+      <c r="S12">
+        <v>1</v>
       </c>
       <c r="V12">
         <v>0</v>
       </c>
       <c r="W12">
-        <v>0.5</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AC12">
-        <v>0.5</v>
-      </c>
-      <c r="AF12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0.5</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0.5</v>
+      </c>
+      <c r="AG12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I13">
+      <c r="J13" s="6">
         <v>0.09</v>
       </c>
-      <c r="J13">
+      <c r="K13" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
+      <c r="S13">
+        <v>1</v>
       </c>
       <c r="V13">
         <v>0</v>
       </c>
       <c r="W13">
-        <v>0.5</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <v>0.5</v>
-      </c>
-      <c r="AF13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0.5</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0.5</v>
+      </c>
+      <c r="AG13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="12">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I14">
+      <c r="J14" s="6">
         <v>0.09</v>
       </c>
-      <c r="J14">
+      <c r="K14" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
+      <c r="S14">
+        <v>1</v>
       </c>
       <c r="V14">
         <v>0</v>
       </c>
       <c r="W14">
-        <v>0.5</v>
-      </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>0.5</v>
-      </c>
-      <c r="AF14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0.5</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0.5</v>
+      </c>
+      <c r="AG14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="12">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I15">
+      <c r="J15" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="J15">
+      <c r="K15" s="6">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
+      <c r="S15">
+        <v>1</v>
       </c>
       <c r="V15">
         <v>0</v>
       </c>
       <c r="W15">
-        <v>0.5</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <v>0.5</v>
-      </c>
-      <c r="AF15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0.5</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0.5</v>
+      </c>
+      <c r="AG15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="12">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I16">
+      <c r="J16" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="J16">
+      <c r="K16" s="6">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
+      <c r="S16">
+        <v>1</v>
       </c>
       <c r="V16">
         <v>0</v>
       </c>
       <c r="W16">
-        <v>0.5</v>
-      </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <v>0.5</v>
-      </c>
-      <c r="AF16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0.5</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0.5</v>
+      </c>
+      <c r="AG16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="12">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="B17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I17">
+      <c r="J17" s="6">
         <v>0.06</v>
       </c>
-      <c r="J17">
+      <c r="K17" s="6">
         <v>0.4</v>
       </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
+      <c r="S17">
+        <v>1</v>
       </c>
       <c r="V17">
         <v>0</v>
       </c>
       <c r="W17">
-        <v>0.5</v>
-      </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AC17">
-        <v>0.5</v>
-      </c>
-      <c r="AF17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0.5</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0.5</v>
+      </c>
+      <c r="AG17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="12">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="B18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I18">
+      <c r="J18" s="6">
         <v>0.06</v>
       </c>
-      <c r="J18">
+      <c r="K18" s="6">
         <v>0.4</v>
       </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
+      <c r="S18">
+        <v>1</v>
       </c>
       <c r="V18">
         <v>0</v>
       </c>
       <c r="W18">
-        <v>0.5</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AC18">
-        <v>0.5</v>
-      </c>
-      <c r="AF18">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0.5</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0.5</v>
+      </c>
+      <c r="AG18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="B19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I19">
+      <c r="J19" s="6">
         <v>0.04</v>
       </c>
-      <c r="J19">
+      <c r="K19" s="6">
         <v>0.13</v>
       </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
+      <c r="S19">
+        <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0.5</v>
-      </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AC19">
-        <v>0.5</v>
-      </c>
-      <c r="AF19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0.5</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0.5</v>
+      </c>
+      <c r="AG19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="12">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="B20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I20">
+      <c r="J20" s="6">
         <v>0.04</v>
       </c>
-      <c r="J20">
+      <c r="K20" s="6">
         <v>0.13</v>
       </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
+      <c r="S20">
+        <v>1</v>
       </c>
       <c r="V20">
         <v>0</v>
       </c>
       <c r="W20">
-        <v>0.5</v>
-      </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AC20">
-        <v>0.5</v>
-      </c>
-      <c r="AF20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0.5</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0.5</v>
+      </c>
+      <c r="AG20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="12">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="B21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I21">
+      <c r="J21" s="6">
         <v>0.08</v>
       </c>
-      <c r="J21">
+      <c r="K21" s="6">
         <v>0.08</v>
       </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
+      <c r="S21">
+        <v>1</v>
       </c>
       <c r="V21">
         <v>0</v>
       </c>
       <c r="W21">
-        <v>0.5</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <v>0.5</v>
-      </c>
-      <c r="AF21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0.5</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0.5</v>
+      </c>
+      <c r="AG21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="12">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I22">
+      <c r="J22" s="6">
         <v>0.08</v>
       </c>
-      <c r="J22">
+      <c r="K22" s="6">
         <v>0.08</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
+      <c r="S22">
+        <v>1</v>
       </c>
       <c r="V22">
         <v>0</v>
       </c>
       <c r="W22">
-        <v>0.5</v>
-      </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AC22">
-        <v>0.5</v>
-      </c>
-      <c r="AF22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0.5</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0.5</v>
+      </c>
+      <c r="AG22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="12">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="B23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I23">
+      <c r="J23" s="6">
         <v>0.06</v>
       </c>
-      <c r="J23">
+      <c r="K23" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
+      <c r="S23">
+        <v>1</v>
       </c>
       <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
         <v>14</v>
       </c>
-      <c r="W23">
-        <v>0.5</v>
-      </c>
-      <c r="Z23">
-        <v>0</v>
-      </c>
-      <c r="AC23">
-        <v>0.5</v>
-      </c>
-      <c r="AF23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="X23">
+        <v>0.5</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0.5</v>
+      </c>
+      <c r="AG23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="12">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="B24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I24">
+      <c r="J24" s="6">
         <v>0.06</v>
       </c>
-      <c r="J24">
+      <c r="K24" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
+      <c r="S24">
+        <v>1</v>
       </c>
       <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
         <v>14</v>
       </c>
-      <c r="W24">
-        <v>0.5</v>
-      </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-      <c r="AC24">
-        <v>0.5</v>
-      </c>
-      <c r="AF24">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="X24">
+        <v>0.5</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0.5</v>
+      </c>
+      <c r="AG24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="12">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="B25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I25">
+      <c r="J25" s="6">
         <v>0.05</v>
       </c>
-      <c r="J25">
+      <c r="K25" s="6">
         <v>0.25</v>
       </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-      <c r="U25">
-        <v>0</v>
+      <c r="S25">
+        <v>1</v>
       </c>
       <c r="V25">
         <v>0</v>
       </c>
       <c r="W25">
-        <v>0.5</v>
-      </c>
-      <c r="Z25">
-        <v>0</v>
-      </c>
-      <c r="AC25">
-        <v>0.5</v>
-      </c>
-      <c r="AF25">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0.5</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0.5</v>
+      </c>
+      <c r="AG25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="12">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="B26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I26">
+      <c r="J26" s="6">
         <v>0.05</v>
       </c>
-      <c r="J26">
+      <c r="K26" s="6">
         <v>0.25</v>
       </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
+      <c r="S26">
+        <v>1</v>
       </c>
       <c r="V26">
         <v>0</v>
       </c>
       <c r="W26">
-        <v>0.5</v>
-      </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AC26">
-        <v>0.5</v>
-      </c>
-      <c r="AF26">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0.5</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0.5</v>
+      </c>
+      <c r="AG26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="12">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="B27" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I27">
+      <c r="J27" s="6">
         <v>0.04</v>
       </c>
-      <c r="J27">
+      <c r="K27" s="6">
         <v>0.01</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>0.04</v>
       </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
+      <c r="S27">
+        <v>1</v>
       </c>
       <c r="V27">
         <v>0</v>
       </c>
       <c r="W27">
-        <v>0.5</v>
-      </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AC27">
-        <v>0.5</v>
-      </c>
-      <c r="AF27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0.5</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0.5</v>
+      </c>
+      <c r="AG27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="12">
-        <v>0</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="B28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I28">
+      <c r="J28" s="6">
         <v>0.04</v>
       </c>
-      <c r="J28">
+      <c r="K28" s="6">
         <v>0.01</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>0.04</v>
       </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-      <c r="U28">
-        <v>0</v>
+      <c r="S28">
+        <v>1</v>
       </c>
       <c r="V28">
         <v>0</v>
       </c>
       <c r="W28">
-        <v>0.5</v>
-      </c>
-      <c r="Z28">
-        <v>0</v>
-      </c>
-      <c r="AC28">
-        <v>0.5</v>
-      </c>
-      <c r="AF28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0.5</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>0.5</v>
+      </c>
+      <c r="AG28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="E29" t="s">
-        <v>11</v>
+      <c r="B29" t="s">
+        <v>24</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="8">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
         <v>58</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>0.03</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>0.01</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>0.05</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>5</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>10</v>
       </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
       <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
         <v>10</v>
       </c>
-      <c r="X29">
-        <v>0.5</v>
-      </c>
       <c r="Y29">
-        <v>1</v>
-      </c>
-      <c r="Z29" s="4" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
-      <c r="AD29">
+      <c r="AC29" s="4"/>
+      <c r="AE29">
         <v>0.995</v>
       </c>
-      <c r="AE29">
-        <v>1</v>
-      </c>
-      <c r="AG29">
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
         <v>0.89</v>
       </c>
-      <c r="AH29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="E30" t="s">
-        <v>11</v>
+      <c r="B30" t="s">
+        <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="8">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
         <v>57</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>0.03</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>0.04</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>10</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="U30">
-        <v>0</v>
-      </c>
       <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
         <v>8</v>
       </c>
-      <c r="X30">
+      <c r="Y30">
         <v>0.6</v>
       </c>
-      <c r="Y30">
+      <c r="Z30">
         <v>0.45</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="E31" t="s">
-        <v>11</v>
+      <c r="B31" t="s">
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="8">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="8">
         <v>2</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>58</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>0.01</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>0.04</v>
       </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
         <v>0.01</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>0.03</v>
-      </c>
-      <c r="S31">
-        <v>50</v>
       </c>
       <c r="T31">
         <v>50</v>
       </c>
       <c r="U31">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
         <v>3</v>
       </c>
-      <c r="X31">
-        <v>1</v>
-      </c>
       <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
         <v>0.52</v>
       </c>
-      <c r="Z31" s="8" t="s">
+      <c r="AA31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AD31">
-        <v>0.5</v>
-      </c>
       <c r="AE31">
-        <v>1</v>
-      </c>
-      <c r="AG31">
-        <v>0.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="AF31">
+        <v>1</v>
       </c>
       <c r="AH31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="AI31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -3884,6 +4089,9 @@
       </c>
       <c r="AH32">
         <v>33</v>
+      </c>
+      <c r="AI32">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>